<commit_message>
Fix bug capex, export by dept
</commit_message>
<xml_diff>
--- a/public/files/Template_Capex_export.xlsx
+++ b/public/files/Template_Capex_export.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\request-budget-master\public\files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7970"/>
   </bookViews>
   <sheets>
     <sheet name="CAPEX" sheetId="1" r:id="rId1"/>
@@ -13,139 +18,139 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
+    <definedName name="__CIP20042">#REF!</definedName>
+    <definedName name="_0201">#REF!</definedName>
+    <definedName name="_8">#REF!</definedName>
+    <definedName name="_CIP20042">#REF!</definedName>
+    <definedName name="acc_acc_code">#REF!</definedName>
+    <definedName name="APR">#REF!</definedName>
+    <definedName name="BRAKE">#REF!</definedName>
+    <definedName name="CALIPER">#REF!</definedName>
+    <definedName name="cc_grn_assy">#REF!</definedName>
+    <definedName name="cc_hdl_assy">#REF!</definedName>
+    <definedName name="cc_prd_body_assy">#REF!</definedName>
+    <definedName name="cc_seat_assy">#REF!</definedName>
+    <definedName name="cost_center_all">#REF!</definedName>
+    <definedName name="cost_center_body">#REF!</definedName>
+    <definedName name="cost_center_unit">#REF!</definedName>
+    <definedName name="CPL_acc_code">#REF!</definedName>
+    <definedName name="CY_Market_Value_of_Equity">#REF!</definedName>
+    <definedName name="CY_Tangible_Net_Worth">#REF!</definedName>
+    <definedName name="CY_Working_Capital">#REF!</definedName>
+    <definedName name="Data_for_Spreadsheet">#REF!</definedName>
+    <definedName name="dert">#REF!</definedName>
     <definedName name="DRUM">#REF!</definedName>
-    <definedName name="kurs_domestic">#REF!</definedName>
-    <definedName name="mte_s_acc_code">#REF!</definedName>
-    <definedName name="mte_acc_code">#REF!</definedName>
-    <definedName name="生产列17">#REF!</definedName>
-    <definedName name="PrintArea">#REF!</definedName>
-    <definedName name="ppb_acc_code">#REF!</definedName>
-    <definedName name="生产期2">#REF!</definedName>
+    <definedName name="enb_acc_code">#REF!</definedName>
+    <definedName name="ENG_BODY">#REF!</definedName>
+    <definedName name="eng_unit">#REF!</definedName>
+    <definedName name="enu_acc_code">#REF!</definedName>
+    <definedName name="fac">#REF!</definedName>
+    <definedName name="fin_acc_code">#REF!</definedName>
+    <definedName name="FRAME">#REF!</definedName>
+    <definedName name="gaf_acc_code">#REF!</definedName>
     <definedName name="gf">#REF!</definedName>
     <definedName name="glklfg">#REF!</definedName>
-    <definedName name="omc_acc_code">#REF!</definedName>
+    <definedName name="HINGE">#REF!</definedName>
+    <definedName name="hrd_acc_code">#REF!</definedName>
+    <definedName name="hrga">#REF!</definedName>
+    <definedName name="irl">#REF!</definedName>
+    <definedName name="irl_acc_code">#REF!</definedName>
+    <definedName name="itd">#REF!</definedName>
+    <definedName name="itd_acc_code">#REF!</definedName>
+    <definedName name="kurs_domestic">#REF!</definedName>
+    <definedName name="kurs_import">#REF!</definedName>
+    <definedName name="LOCK">#REF!</definedName>
     <definedName name="mkt">#REF!</definedName>
-    <definedName name="_0201">#REF!</definedName>
-    <definedName name="enb_acc_code">#REF!</definedName>
-    <definedName name="Spec">#REF!</definedName>
-    <definedName name="T_capextype">#REF!</definedName>
-    <definedName name="APR">#REF!</definedName>
-    <definedName name="cc_hdl_assy">#REF!</definedName>
-    <definedName name="qa_unit">#REF!</definedName>
-    <definedName name="itd_acc_code">#REF!</definedName>
-    <definedName name="__CIP20042">#REF!</definedName>
-    <definedName name="profit_center_unit">#REF!</definedName>
-    <definedName name="生产期17">#REF!</definedName>
-    <definedName name="ppic">#REF!</definedName>
-    <definedName name="profit_center_body">#REF!</definedName>
-    <definedName name="hrga">#REF!</definedName>
-    <definedName name="irl_acc_code">#REF!</definedName>
-    <definedName name="汇率">#REF!</definedName>
-    <definedName name="acc_acc_code">#REF!</definedName>
-    <definedName name="生产期9">#REF!</definedName>
-    <definedName name="cc_grn_assy">#REF!</definedName>
-    <definedName name="qa_body">#REF!</definedName>
-    <definedName name="omc">#REF!</definedName>
-    <definedName name="profit_center_admin">#REF!</definedName>
-    <definedName name="生产期1">#REF!</definedName>
-    <definedName name="fac">#REF!</definedName>
-    <definedName name="fin_acc_code">#REF!</definedName>
-    <definedName name="生产期16">#REF!</definedName>
-    <definedName name="pru_acc_code">#REF!</definedName>
-    <definedName name="HINGE">#REF!</definedName>
-    <definedName name="生产列4">#REF!</definedName>
-    <definedName name="qab_acc_code">#REF!</definedName>
-    <definedName name="LOCK">#REF!</definedName>
-    <definedName name="cost_center_unit">#REF!</definedName>
-    <definedName name="生产列15">#REF!</definedName>
-    <definedName name="qa_system">#REF!</definedName>
-    <definedName name="PY2_Retained_Earnings">#REF!</definedName>
-    <definedName name="kurs_import">#REF!</definedName>
-    <definedName name="T_costcenter">#REF!</definedName>
-    <definedName name="ENG_BODY">#REF!</definedName>
-    <definedName name="UFPrn20050811133035">#REF!</definedName>
-    <definedName name="cost_center_body">#REF!</definedName>
-    <definedName name="eng_unit">#REF!</definedName>
-    <definedName name="生产列7">#REF!</definedName>
-    <definedName name="生产期6">#REF!</definedName>
-    <definedName name="tabel_dept">#REF!</definedName>
-    <definedName name="WPOP">#REF!</definedName>
-    <definedName name="生产列9">#REF!</definedName>
-    <definedName name="mte_m_acc_code">#REF!</definedName>
-    <definedName name="PY2_Tangible_Net_Worth">#REF!</definedName>
-    <definedName name="profit_center_all">#REF!</definedName>
-    <definedName name="生产期19">#REF!</definedName>
-    <definedName name="CY_Working_Capital">#REF!</definedName>
-    <definedName name="生产期3">#REF!</definedName>
-    <definedName name="CY_Market_Value_of_Equity">#REF!</definedName>
-    <definedName name="PY_Market_Value_of_Equity">#REF!</definedName>
-    <definedName name="prd_body">#REF!</definedName>
-    <definedName name="PY_Working_Capital">#REF!</definedName>
-    <definedName name="mte_e_acc_code">#REF!</definedName>
-    <definedName name="qas_acc_code">#REF!</definedName>
-    <definedName name="mte_d_acc_code">#REF!</definedName>
-    <definedName name="cc_seat_assy">#REF!</definedName>
-    <definedName name="生产列8">#REF!</definedName>
-    <definedName name="PY2_Working_Capital">#REF!</definedName>
-    <definedName name="生产列11">#REF!</definedName>
-    <definedName name="enu_acc_code">#REF!</definedName>
-    <definedName name="生产期20">#REF!</definedName>
-    <definedName name="FRAME">#REF!</definedName>
-    <definedName name="生产期8">#REF!</definedName>
-    <definedName name="生产列16">#REF!</definedName>
     <definedName name="mkt_acc_code">#REF!</definedName>
-    <definedName name="gaf_acc_code">#REF!</definedName>
-    <definedName name="BRAKE">#REF!</definedName>
-    <definedName name="CALIPER">#REF!</definedName>
-    <definedName name="生产列20">#REF!</definedName>
     <definedName name="MOLD">#REF!</definedName>
     <definedName name="mte">#REF!</definedName>
-    <definedName name="CPL_acc_code">#REF!</definedName>
-    <definedName name="irl">#REF!</definedName>
+    <definedName name="mte_acc_code">#REF!</definedName>
+    <definedName name="mte_d_acc_code">#REF!</definedName>
+    <definedName name="mte_e_acc_code">#REF!</definedName>
+    <definedName name="mte_m_acc_code">#REF!</definedName>
+    <definedName name="mte_s_acc_code">#REF!</definedName>
+    <definedName name="omc">#REF!</definedName>
+    <definedName name="omc_acc_code">#REF!</definedName>
+    <definedName name="PKG">#REF!</definedName>
+    <definedName name="PLAN">#REF!</definedName>
+    <definedName name="ppb_acc_code">#REF!</definedName>
+    <definedName name="ppc_acc_code">#REF!</definedName>
+    <definedName name="ppic">#REF!</definedName>
+    <definedName name="ppu_acc_code">#REF!</definedName>
+    <definedName name="prb_acc_code">#REF!</definedName>
+    <definedName name="prd_body">#REF!</definedName>
+    <definedName name="prd_unit">#REF!</definedName>
+    <definedName name="Print_Area_MI">#REF!</definedName>
+    <definedName name="PrintArea">#REF!</definedName>
+    <definedName name="profit_center_admin">#REF!</definedName>
+    <definedName name="profit_center_all">#REF!</definedName>
+    <definedName name="profit_center_body">#REF!</definedName>
+    <definedName name="profit_center_unit">#REF!</definedName>
+    <definedName name="pru_acc_code">#REF!</definedName>
+    <definedName name="pur">#REF!</definedName>
+    <definedName name="pur_acc_code">#REF!</definedName>
+    <definedName name="PY_Market_Value_of_Equity">#REF!</definedName>
+    <definedName name="PY_Tangible_Net_Worth">#REF!</definedName>
+    <definedName name="PY_Working_Capital">#REF!</definedName>
+    <definedName name="PY2_Retained_Earnings">#REF!</definedName>
+    <definedName name="PY2_Tangible_Net_Worth">#REF!</definedName>
+    <definedName name="PY2_Working_Capital">#REF!</definedName>
+    <definedName name="qa_body">#REF!</definedName>
+    <definedName name="qa_system">#REF!</definedName>
+    <definedName name="qa_unit">#REF!</definedName>
+    <definedName name="qab_acc_code">#REF!</definedName>
+    <definedName name="qas_acc_code">#REF!</definedName>
+    <definedName name="qau_acc_code">#REF!</definedName>
+    <definedName name="Report">#REF!</definedName>
+    <definedName name="SEPT">#REF!</definedName>
+    <definedName name="Spec">#REF!</definedName>
+    <definedName name="STOTAL">#REF!</definedName>
+    <definedName name="T_capextype">#REF!</definedName>
+    <definedName name="T_costcenter">#REF!</definedName>
     <definedName name="T_currency">#REF!</definedName>
+    <definedName name="T_impdom">#REF!</definedName>
+    <definedName name="T_periode">#REF!</definedName>
+    <definedName name="T_profitcenter">#REF!</definedName>
+    <definedName name="T_profitcode">#REF!</definedName>
+    <definedName name="tabel_dept">#REF!</definedName>
+    <definedName name="TOTAL">#REF!</definedName>
+    <definedName name="UFPrn20050811133035">#REF!</definedName>
+    <definedName name="VAND">#REF!</definedName>
+    <definedName name="WPOP">#REF!</definedName>
+    <definedName name="汇率">#REF!</definedName>
+    <definedName name="生产列1">#REF!</definedName>
+    <definedName name="生产列11">#REF!</definedName>
+    <definedName name="生产列15">#REF!</definedName>
+    <definedName name="生产列16">#REF!</definedName>
+    <definedName name="生产列17">#REF!</definedName>
+    <definedName name="生产列19">#REF!</definedName>
+    <definedName name="生产列2">#REF!</definedName>
+    <definedName name="生产列20">#REF!</definedName>
+    <definedName name="生产列3">#REF!</definedName>
+    <definedName name="生产列4">#REF!</definedName>
+    <definedName name="生产列5">#REF!</definedName>
+    <definedName name="生产列6">#REF!</definedName>
+    <definedName name="生产列7">#REF!</definedName>
+    <definedName name="生产列8">#REF!</definedName>
+    <definedName name="生产列9">#REF!</definedName>
+    <definedName name="生产期">#REF!</definedName>
+    <definedName name="生产期1">#REF!</definedName>
+    <definedName name="生产期11">#REF!</definedName>
+    <definedName name="生产期15">#REF!</definedName>
+    <definedName name="生产期16">#REF!</definedName>
+    <definedName name="生产期17">#REF!</definedName>
+    <definedName name="生产期19">#REF!</definedName>
+    <definedName name="生产期2">#REF!</definedName>
+    <definedName name="生产期20">#REF!</definedName>
+    <definedName name="生产期3">#REF!</definedName>
+    <definedName name="生产期4">#REF!</definedName>
     <definedName name="生产期5">#REF!</definedName>
-    <definedName name="Report">#REF!</definedName>
-    <definedName name="T_profitcenter">#REF!</definedName>
-    <definedName name="itd">#REF!</definedName>
-    <definedName name="ppu_acc_code">#REF!</definedName>
-    <definedName name="_8">#REF!</definedName>
-    <definedName name="qau_acc_code">#REF!</definedName>
-    <definedName name="生产期11">#REF!</definedName>
-    <definedName name="生产列1">#REF!</definedName>
-    <definedName name="pur">#REF!</definedName>
-    <definedName name="STOTAL">#REF!</definedName>
-    <definedName name="TOTAL">#REF!</definedName>
-    <definedName name="生产列6">#REF!</definedName>
-    <definedName name="生产列19">#REF!</definedName>
-    <definedName name="SEPT">#REF!</definedName>
-    <definedName name="Print_Area_MI">#REF!</definedName>
-    <definedName name="T_profitcode">#REF!</definedName>
-    <definedName name="生产期15">#REF!</definedName>
-    <definedName name="VAND">#REF!</definedName>
-    <definedName name="生产列3">#REF!</definedName>
-    <definedName name="生产期">#REF!</definedName>
-    <definedName name="_CIP20042">#REF!</definedName>
-    <definedName name="cc_prd_body_assy">#REF!</definedName>
-    <definedName name="生产期4">#REF!</definedName>
-    <definedName name="PKG">#REF!</definedName>
-    <definedName name="T_impdom">#REF!</definedName>
-    <definedName name="生产列5">#REF!</definedName>
-    <definedName name="hrd_acc_code">#REF!</definedName>
-    <definedName name="prb_acc_code">#REF!</definedName>
-    <definedName name="dert">#REF!</definedName>
-    <definedName name="pur_acc_code">#REF!</definedName>
-    <definedName name="prd_unit">#REF!</definedName>
-    <definedName name="ppc_acc_code">#REF!</definedName>
-    <definedName name="cost_center_all">#REF!</definedName>
-    <definedName name="CY_Tangible_Net_Worth">#REF!</definedName>
+    <definedName name="生产期6">#REF!</definedName>
     <definedName name="生产期7">#REF!</definedName>
-    <definedName name="PY_Tangible_Net_Worth">#REF!</definedName>
-    <definedName name="PLAN">#REF!</definedName>
-    <definedName name="Data_for_Spreadsheet">#REF!</definedName>
-    <definedName name="生产列2">#REF!</definedName>
-    <definedName name="T_periode">#REF!</definedName>
+    <definedName name="生产期8">#REF!</definedName>
+    <definedName name="生产期9">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -285,19 +290,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="9">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@"/>
-    <numFmt numFmtId="180" formatCode="[$-409]mmm\-yy"/>
-    <numFmt numFmtId="181" formatCode="0.0%"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="5">
+    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@"/>
+    <numFmt numFmtId="170" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@"/>
+    <numFmt numFmtId="171" formatCode="[$-409]mmm\-yy"/>
+    <numFmt numFmtId="172" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,152 +346,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="37">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -521,194 +378,8 @@
         <bgColor rgb="FFFFE598"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="18">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -825,251 +496,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1100,17 +529,17 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="180" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1127,76 +556,50 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="181" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="181" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="181" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="181" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="181" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1214,13 +617,23 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="#REF"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
 </externalLink>
 </file>
 
@@ -1416,60 +829,61 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:AO1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:X3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="14.5714285714286" customWidth="1"/>
-    <col min="3" max="3" width="9.57142857142857" customWidth="1"/>
-    <col min="4" max="4" width="23.1428571428571" customWidth="1"/>
-    <col min="5" max="5" width="24.4285714285714" customWidth="1"/>
-    <col min="6" max="6" width="18.5714285714286" customWidth="1"/>
-    <col min="7" max="7" width="12.4285714285714" customWidth="1"/>
-    <col min="8" max="8" width="23.4285714285714" customWidth="1"/>
-    <col min="9" max="10" width="18.1428571428571" customWidth="1"/>
-    <col min="11" max="11" width="13.8571428571429" customWidth="1"/>
-    <col min="12" max="12" width="44.4285714285714" customWidth="1"/>
-    <col min="13" max="13" width="25.4285714285714" customWidth="1"/>
-    <col min="14" max="14" width="6.85714285714286" customWidth="1"/>
-    <col min="15" max="15" width="13.8571428571429" customWidth="1"/>
-    <col min="16" max="16" width="18.5714285714286" customWidth="1"/>
+    <col min="1" max="2" width="14.54296875" customWidth="1"/>
+    <col min="3" max="3" width="9.54296875" customWidth="1"/>
+    <col min="4" max="4" width="23.1796875" customWidth="1"/>
+    <col min="5" max="5" width="24.453125" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" customWidth="1"/>
+    <col min="8" max="8" width="23.453125" customWidth="1"/>
+    <col min="9" max="10" width="18.1796875" customWidth="1"/>
+    <col min="11" max="11" width="13.81640625" customWidth="1"/>
+    <col min="12" max="12" width="44.453125" customWidth="1"/>
+    <col min="13" max="13" width="25.453125" customWidth="1"/>
+    <col min="14" max="14" width="6.81640625" customWidth="1"/>
+    <col min="15" max="15" width="13.81640625" customWidth="1"/>
+    <col min="16" max="16" width="18.54296875" customWidth="1"/>
     <col min="17" max="17" width="15" customWidth="1"/>
     <col min="18" max="18" width="16" customWidth="1"/>
-    <col min="19" max="20" width="19.4285714285714" customWidth="1"/>
-    <col min="21" max="21" width="14.4285714285714" customWidth="1"/>
-    <col min="22" max="22" width="19.4285714285714" customWidth="1"/>
-    <col min="23" max="24" width="14.4285714285714" customWidth="1"/>
-    <col min="25" max="26" width="9.85714285714286" customWidth="1"/>
+    <col min="19" max="20" width="19.453125" customWidth="1"/>
+    <col min="21" max="21" width="14.453125" customWidth="1"/>
+    <col min="22" max="22" width="19.453125" customWidth="1"/>
+    <col min="23" max="24" width="14.453125" customWidth="1"/>
+    <col min="25" max="26" width="9.81640625" customWidth="1"/>
     <col min="27" max="27" width="9" customWidth="1"/>
-    <col min="28" max="28" width="8.42857142857143" customWidth="1"/>
-    <col min="29" max="29" width="9.71428571428571" customWidth="1"/>
-    <col min="30" max="30" width="9.42857142857143" customWidth="1"/>
-    <col min="31" max="31" width="8.71428571428571" customWidth="1"/>
-    <col min="32" max="32" width="9.71428571428571" customWidth="1"/>
-    <col min="33" max="34" width="9.42857142857143" customWidth="1"/>
-    <col min="35" max="35" width="9.85714285714286" customWidth="1"/>
-    <col min="36" max="36" width="10.1428571428571" customWidth="1"/>
-    <col min="37" max="37" width="8.71428571428571" customWidth="1"/>
-    <col min="38" max="38" width="5.42857142857143" customWidth="1"/>
-    <col min="39" max="39" width="50.5714285714286" customWidth="1"/>
+    <col min="28" max="28" width="8.453125" customWidth="1"/>
+    <col min="29" max="29" width="9.7265625" customWidth="1"/>
+    <col min="30" max="30" width="9.453125" customWidth="1"/>
+    <col min="31" max="31" width="8.7265625" customWidth="1"/>
+    <col min="32" max="32" width="9.7265625" customWidth="1"/>
+    <col min="33" max="34" width="9.453125" customWidth="1"/>
+    <col min="35" max="35" width="9.81640625" customWidth="1"/>
+    <col min="36" max="36" width="10.1796875" customWidth="1"/>
+    <col min="37" max="37" width="8.7265625" customWidth="1"/>
+    <col min="38" max="38" width="5.453125" customWidth="1"/>
+    <col min="39" max="39" width="50.54296875" customWidth="1"/>
     <col min="40" max="40" width="19" customWidth="1"/>
-    <col min="41" max="41" width="9.14285714285714" customWidth="1"/>
+    <col min="41" max="41" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="49.5" customHeight="1" spans="2:36">
+    <row r="1" spans="1:36" ht="49.5" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1576,7 +990,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" ht="39.75" customHeight="1" spans="1:36">
+    <row r="2" spans="1:36" ht="39.75" customHeight="1">
       <c r="A2" s="6"/>
       <c r="B2" s="7" t="s">
         <v>35</v>
@@ -1618,7 +1032,7 @@
       <c r="AI2" s="19"/>
       <c r="AJ2" s="19"/>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:36" ht="14.5">
       <c r="A3" s="6"/>
       <c r="C3" s="8">
         <v>2</v>
@@ -1657,7 +1071,7 @@
       <c r="AI3" s="19"/>
       <c r="AJ3" s="19"/>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:36" ht="14.5">
       <c r="A4" s="6"/>
       <c r="C4" s="8">
         <v>3</v>
@@ -1676,17 +1090,13 @@
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
-      <c r="N4" s="9">
-        <v>1</v>
-      </c>
+      <c r="N4" s="9"/>
       <c r="O4" s="10"/>
       <c r="P4" s="13"/>
       <c r="Q4" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R4" s="16">
-        <v>0</v>
-      </c>
+      <c r="R4" s="16"/>
       <c r="S4" s="17"/>
       <c r="T4" s="17"/>
       <c r="U4" s="13"/>
@@ -1706,7 +1116,7 @@
       <c r="AI4" s="19"/>
       <c r="AJ4" s="19"/>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:36" ht="14.5">
       <c r="A5" s="6"/>
       <c r="C5" s="8">
         <v>4</v>
@@ -1725,17 +1135,13 @@
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
-      <c r="N5" s="9">
-        <v>1</v>
-      </c>
+      <c r="N5" s="9"/>
       <c r="O5" s="10"/>
       <c r="P5" s="13"/>
       <c r="Q5" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R5" s="16">
-        <v>0</v>
-      </c>
+      <c r="R5" s="16"/>
       <c r="S5" s="17"/>
       <c r="T5" s="17"/>
       <c r="U5" s="13"/>
@@ -1755,7 +1161,7 @@
       <c r="AI5" s="19"/>
       <c r="AJ5" s="19"/>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:36" ht="14.5">
       <c r="A6" s="6"/>
       <c r="C6" s="8">
         <v>5</v>
@@ -1774,17 +1180,13 @@
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
-      <c r="N6" s="9">
-        <v>1</v>
-      </c>
+      <c r="N6" s="9"/>
       <c r="O6" s="10"/>
       <c r="P6" s="13"/>
       <c r="Q6" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R6" s="16">
-        <v>0</v>
-      </c>
+      <c r="R6" s="16"/>
       <c r="S6" s="17"/>
       <c r="T6" s="17"/>
       <c r="U6" s="13"/>
@@ -1804,7 +1206,7 @@
       <c r="AI6" s="19"/>
       <c r="AJ6" s="19"/>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:36" ht="14.5">
       <c r="A7" s="6"/>
       <c r="C7" s="8">
         <v>6</v>
@@ -1823,17 +1225,13 @@
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
-      <c r="N7" s="9">
-        <v>1</v>
-      </c>
+      <c r="N7" s="9"/>
       <c r="O7" s="10"/>
       <c r="P7" s="13"/>
       <c r="Q7" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R7" s="16">
-        <v>0</v>
-      </c>
+      <c r="R7" s="16"/>
       <c r="S7" s="17"/>
       <c r="T7" s="17"/>
       <c r="U7" s="13"/>
@@ -1853,7 +1251,7 @@
       <c r="AI7" s="19"/>
       <c r="AJ7" s="19"/>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:36" ht="14.5">
       <c r="A8" s="6"/>
       <c r="C8" s="8">
         <v>7</v>
@@ -1872,17 +1270,13 @@
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
-      <c r="N8" s="9">
-        <v>1</v>
-      </c>
+      <c r="N8" s="9"/>
       <c r="O8" s="10"/>
       <c r="P8" s="13"/>
       <c r="Q8" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R8" s="16">
-        <v>0</v>
-      </c>
+      <c r="R8" s="16"/>
       <c r="S8" s="17"/>
       <c r="T8" s="17"/>
       <c r="U8" s="13"/>
@@ -1902,7 +1296,7 @@
       <c r="AI8" s="19"/>
       <c r="AJ8" s="19"/>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:36" ht="14.5">
       <c r="A9" s="6"/>
       <c r="C9" s="8">
         <v>8</v>
@@ -1921,17 +1315,13 @@
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
-      <c r="N9" s="9">
-        <v>1</v>
-      </c>
+      <c r="N9" s="9"/>
       <c r="O9" s="10"/>
       <c r="P9" s="13"/>
       <c r="Q9" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R9" s="16">
-        <v>0</v>
-      </c>
+      <c r="R9" s="16"/>
       <c r="S9" s="17"/>
       <c r="T9" s="17"/>
       <c r="U9" s="13"/>
@@ -1951,7 +1341,7 @@
       <c r="AI9" s="19"/>
       <c r="AJ9" s="19"/>
     </row>
-    <row r="10" spans="1:36">
+    <row r="10" spans="1:36" ht="14.5">
       <c r="A10" s="6"/>
       <c r="C10" s="8">
         <v>9</v>
@@ -1970,17 +1360,13 @@
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
-      <c r="N10" s="9">
-        <v>1</v>
-      </c>
+      <c r="N10" s="9"/>
       <c r="O10" s="10"/>
       <c r="P10" s="13"/>
       <c r="Q10" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R10" s="16">
-        <v>0</v>
-      </c>
+      <c r="R10" s="16"/>
       <c r="S10" s="17"/>
       <c r="T10" s="17"/>
       <c r="U10" s="13"/>
@@ -2000,7 +1386,7 @@
       <c r="AI10" s="19"/>
       <c r="AJ10" s="19"/>
     </row>
-    <row r="11" spans="1:36">
+    <row r="11" spans="1:36" ht="14.5">
       <c r="A11" s="6"/>
       <c r="C11" s="8">
         <v>10</v>
@@ -2019,17 +1405,13 @@
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
-      <c r="N11" s="9">
-        <v>1</v>
-      </c>
+      <c r="N11" s="9"/>
       <c r="O11" s="10"/>
       <c r="P11" s="13"/>
       <c r="Q11" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R11" s="16">
-        <v>0</v>
-      </c>
+      <c r="R11" s="16"/>
       <c r="S11" s="17"/>
       <c r="T11" s="17"/>
       <c r="U11" s="13"/>
@@ -2049,7 +1431,7 @@
       <c r="AI11" s="19"/>
       <c r="AJ11" s="19"/>
     </row>
-    <row r="12" spans="1:36">
+    <row r="12" spans="1:36" ht="14.5">
       <c r="A12" s="6"/>
       <c r="C12" s="8">
         <v>11</v>
@@ -2068,17 +1450,13 @@
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
-      <c r="N12" s="9">
-        <v>1</v>
-      </c>
+      <c r="N12" s="9"/>
       <c r="O12" s="10"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R12" s="16">
-        <v>0</v>
-      </c>
+      <c r="R12" s="16"/>
       <c r="S12" s="17"/>
       <c r="T12" s="17"/>
       <c r="U12" s="13"/>
@@ -2098,7 +1476,7 @@
       <c r="AI12" s="19"/>
       <c r="AJ12" s="19"/>
     </row>
-    <row r="13" spans="1:36">
+    <row r="13" spans="1:36" ht="14.5">
       <c r="A13" s="6"/>
       <c r="C13" s="8">
         <v>12</v>
@@ -2117,17 +1495,13 @@
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
-      <c r="N13" s="9">
-        <v>1</v>
-      </c>
+      <c r="N13" s="9"/>
       <c r="O13" s="10"/>
       <c r="P13" s="13"/>
       <c r="Q13" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R13" s="16">
-        <v>0</v>
-      </c>
+      <c r="R13" s="16"/>
       <c r="S13" s="17"/>
       <c r="T13" s="17"/>
       <c r="U13" s="13"/>
@@ -2147,7 +1521,7 @@
       <c r="AI13" s="19"/>
       <c r="AJ13" s="19"/>
     </row>
-    <row r="14" spans="1:36">
+    <row r="14" spans="1:36" ht="14.5">
       <c r="A14" s="6"/>
       <c r="C14" s="8">
         <v>13</v>
@@ -2166,17 +1540,13 @@
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
-      <c r="N14" s="9">
-        <v>1</v>
-      </c>
+      <c r="N14" s="9"/>
       <c r="O14" s="10"/>
       <c r="P14" s="13"/>
       <c r="Q14" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R14" s="16">
-        <v>0</v>
-      </c>
+      <c r="R14" s="16"/>
       <c r="S14" s="17"/>
       <c r="T14" s="17"/>
       <c r="U14" s="13"/>
@@ -2196,7 +1566,7 @@
       <c r="AI14" s="19"/>
       <c r="AJ14" s="19"/>
     </row>
-    <row r="15" spans="1:36">
+    <row r="15" spans="1:36" ht="14.5">
       <c r="A15" s="6"/>
       <c r="C15" s="8">
         <v>14</v>
@@ -2215,17 +1585,13 @@
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
-      <c r="N15" s="9">
-        <v>1</v>
-      </c>
+      <c r="N15" s="9"/>
       <c r="O15" s="10"/>
       <c r="P15" s="13"/>
       <c r="Q15" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R15" s="16">
-        <v>0</v>
-      </c>
+      <c r="R15" s="16"/>
       <c r="S15" s="17"/>
       <c r="T15" s="17"/>
       <c r="U15" s="13"/>
@@ -2245,7 +1611,7 @@
       <c r="AI15" s="19"/>
       <c r="AJ15" s="19"/>
     </row>
-    <row r="16" spans="1:36">
+    <row r="16" spans="1:36" ht="14.5">
       <c r="A16" s="6"/>
       <c r="C16" s="8">
         <v>15</v>
@@ -2264,17 +1630,13 @@
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
-      <c r="N16" s="9">
-        <v>1</v>
-      </c>
+      <c r="N16" s="9"/>
       <c r="O16" s="10"/>
       <c r="P16" s="13"/>
       <c r="Q16" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R16" s="16">
-        <v>0</v>
-      </c>
+      <c r="R16" s="16"/>
       <c r="S16" s="17"/>
       <c r="T16" s="17"/>
       <c r="U16" s="13"/>
@@ -2294,7 +1656,7 @@
       <c r="AI16" s="19"/>
       <c r="AJ16" s="19"/>
     </row>
-    <row r="17" spans="1:36">
+    <row r="17" spans="1:36" ht="14.5">
       <c r="A17" s="6"/>
       <c r="C17" s="8">
         <v>16</v>
@@ -2313,17 +1675,13 @@
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
-      <c r="N17" s="9">
-        <v>1</v>
-      </c>
+      <c r="N17" s="9"/>
       <c r="O17" s="10"/>
       <c r="P17" s="13"/>
       <c r="Q17" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R17" s="16">
-        <v>0</v>
-      </c>
+      <c r="R17" s="16"/>
       <c r="S17" s="17"/>
       <c r="T17" s="17"/>
       <c r="U17" s="13"/>
@@ -2343,7 +1701,7 @@
       <c r="AI17" s="19"/>
       <c r="AJ17" s="19"/>
     </row>
-    <row r="18" spans="1:36">
+    <row r="18" spans="1:36" ht="14.5">
       <c r="A18" s="6"/>
       <c r="C18" s="8">
         <v>17</v>
@@ -2362,17 +1720,13 @@
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
-      <c r="N18" s="9">
-        <v>1</v>
-      </c>
+      <c r="N18" s="9"/>
       <c r="O18" s="10"/>
       <c r="P18" s="13"/>
       <c r="Q18" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R18" s="16">
-        <v>0</v>
-      </c>
+      <c r="R18" s="16"/>
       <c r="S18" s="17"/>
       <c r="T18" s="17"/>
       <c r="U18" s="13"/>
@@ -2392,7 +1746,7 @@
       <c r="AI18" s="19"/>
       <c r="AJ18" s="19"/>
     </row>
-    <row r="19" spans="1:36">
+    <row r="19" spans="1:36" ht="14.5">
       <c r="A19" s="6"/>
       <c r="C19" s="8">
         <v>18</v>
@@ -2411,17 +1765,13 @@
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
-      <c r="N19" s="9">
-        <v>1</v>
-      </c>
+      <c r="N19" s="9"/>
       <c r="O19" s="10"/>
       <c r="P19" s="13"/>
       <c r="Q19" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R19" s="16">
-        <v>0</v>
-      </c>
+      <c r="R19" s="16"/>
       <c r="S19" s="17"/>
       <c r="T19" s="17"/>
       <c r="U19" s="13"/>
@@ -2441,7 +1791,7 @@
       <c r="AI19" s="19"/>
       <c r="AJ19" s="19"/>
     </row>
-    <row r="20" spans="1:36">
+    <row r="20" spans="1:36" ht="14.5">
       <c r="A20" s="6"/>
       <c r="C20" s="8">
         <v>19</v>
@@ -2460,17 +1810,13 @@
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
-      <c r="N20" s="9">
-        <v>1</v>
-      </c>
+      <c r="N20" s="9"/>
       <c r="O20" s="10"/>
       <c r="P20" s="13"/>
       <c r="Q20" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R20" s="16">
-        <v>0</v>
-      </c>
+      <c r="R20" s="16"/>
       <c r="S20" s="17"/>
       <c r="T20" s="17"/>
       <c r="U20" s="13"/>
@@ -2490,7 +1836,7 @@
       <c r="AI20" s="19"/>
       <c r="AJ20" s="19"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1" spans="1:36">
+    <row r="21" spans="1:36" ht="15.75" customHeight="1">
       <c r="A21" s="6"/>
       <c r="C21" s="8">
         <v>20</v>
@@ -2509,17 +1855,13 @@
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
-      <c r="N21" s="9">
-        <v>1</v>
-      </c>
+      <c r="N21" s="9"/>
       <c r="O21" s="10"/>
       <c r="P21" s="13"/>
       <c r="Q21" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R21" s="16">
-        <v>0</v>
-      </c>
+      <c r="R21" s="16"/>
       <c r="S21" s="17"/>
       <c r="T21" s="17"/>
       <c r="U21" s="13"/>
@@ -2539,7 +1881,7 @@
       <c r="AI21" s="19"/>
       <c r="AJ21" s="19"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1" spans="1:36">
+    <row r="22" spans="1:36" ht="15.75" customHeight="1">
       <c r="A22" s="6"/>
       <c r="C22" s="8">
         <v>21</v>
@@ -2558,17 +1900,13 @@
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
-      <c r="N22" s="9">
-        <v>1</v>
-      </c>
+      <c r="N22" s="9"/>
       <c r="O22" s="10"/>
       <c r="P22" s="13"/>
       <c r="Q22" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R22" s="16">
-        <v>0</v>
-      </c>
+      <c r="R22" s="16"/>
       <c r="S22" s="17"/>
       <c r="T22" s="17"/>
       <c r="U22" s="13"/>
@@ -2588,7 +1926,7 @@
       <c r="AI22" s="19"/>
       <c r="AJ22" s="19"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1" spans="1:36">
+    <row r="23" spans="1:36" ht="15.75" customHeight="1">
       <c r="A23" s="6"/>
       <c r="C23" s="8">
         <v>22</v>
@@ -2607,17 +1945,13 @@
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
       <c r="M23" s="10"/>
-      <c r="N23" s="9">
-        <v>1</v>
-      </c>
+      <c r="N23" s="9"/>
       <c r="O23" s="10"/>
       <c r="P23" s="13"/>
       <c r="Q23" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R23" s="16">
-        <v>0</v>
-      </c>
+      <c r="R23" s="16"/>
       <c r="S23" s="17"/>
       <c r="T23" s="17"/>
       <c r="U23" s="13"/>
@@ -2637,7 +1971,7 @@
       <c r="AI23" s="19"/>
       <c r="AJ23" s="19"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1" spans="1:36">
+    <row r="24" spans="1:36" ht="15.75" customHeight="1">
       <c r="A24" s="6"/>
       <c r="C24" s="8">
         <v>23</v>
@@ -2656,17 +1990,13 @@
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
       <c r="M24" s="10"/>
-      <c r="N24" s="9">
-        <v>1</v>
-      </c>
+      <c r="N24" s="9"/>
       <c r="O24" s="10"/>
       <c r="P24" s="13"/>
       <c r="Q24" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R24" s="16">
-        <v>0</v>
-      </c>
+      <c r="R24" s="16"/>
       <c r="S24" s="17"/>
       <c r="T24" s="17"/>
       <c r="U24" s="13"/>
@@ -2686,7 +2016,7 @@
       <c r="AI24" s="19"/>
       <c r="AJ24" s="19"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1" spans="1:36">
+    <row r="25" spans="1:36" ht="15.75" customHeight="1">
       <c r="A25" s="6"/>
       <c r="C25" s="8">
         <v>24</v>
@@ -2705,17 +2035,13 @@
       <c r="K25" s="10"/>
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
-      <c r="N25" s="9">
-        <v>1</v>
-      </c>
+      <c r="N25" s="9"/>
       <c r="O25" s="10"/>
       <c r="P25" s="13"/>
       <c r="Q25" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R25" s="16">
-        <v>0</v>
-      </c>
+      <c r="R25" s="16"/>
       <c r="S25" s="17"/>
       <c r="T25" s="17"/>
       <c r="U25" s="13"/>
@@ -2735,7 +2061,7 @@
       <c r="AI25" s="19"/>
       <c r="AJ25" s="19"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1" spans="1:36">
+    <row r="26" spans="1:36" ht="15.75" customHeight="1">
       <c r="A26" s="6"/>
       <c r="C26" s="8">
         <v>25</v>
@@ -2754,17 +2080,13 @@
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
-      <c r="N26" s="9">
-        <v>1</v>
-      </c>
+      <c r="N26" s="9"/>
       <c r="O26" s="10"/>
       <c r="P26" s="13"/>
       <c r="Q26" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R26" s="16">
-        <v>0</v>
-      </c>
+      <c r="R26" s="16"/>
       <c r="S26" s="17"/>
       <c r="T26" s="17"/>
       <c r="U26" s="13"/>
@@ -2784,7 +2106,7 @@
       <c r="AI26" s="19"/>
       <c r="AJ26" s="19"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1" spans="1:36">
+    <row r="27" spans="1:36" ht="15.75" customHeight="1">
       <c r="A27" s="6"/>
       <c r="C27" s="8">
         <v>26</v>
@@ -2803,17 +2125,13 @@
       <c r="K27" s="10"/>
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
-      <c r="N27" s="9">
-        <v>1</v>
-      </c>
+      <c r="N27" s="9"/>
       <c r="O27" s="10"/>
       <c r="P27" s="13"/>
       <c r="Q27" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R27" s="16">
-        <v>0</v>
-      </c>
+      <c r="R27" s="16"/>
       <c r="S27" s="17"/>
       <c r="T27" s="17"/>
       <c r="U27" s="13"/>
@@ -2833,7 +2151,7 @@
       <c r="AI27" s="19"/>
       <c r="AJ27" s="19"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1" spans="1:36">
+    <row r="28" spans="1:36" ht="15.75" customHeight="1">
       <c r="A28" s="6"/>
       <c r="C28" s="8">
         <v>27</v>
@@ -2852,17 +2170,13 @@
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
       <c r="M28" s="10"/>
-      <c r="N28" s="9">
-        <v>1</v>
-      </c>
+      <c r="N28" s="9"/>
       <c r="O28" s="10"/>
       <c r="P28" s="13"/>
       <c r="Q28" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R28" s="16">
-        <v>0</v>
-      </c>
+      <c r="R28" s="16"/>
       <c r="S28" s="17"/>
       <c r="T28" s="17"/>
       <c r="U28" s="13"/>
@@ -2882,7 +2196,7 @@
       <c r="AI28" s="19"/>
       <c r="AJ28" s="19"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1" spans="1:36">
+    <row r="29" spans="1:36" ht="15.75" customHeight="1">
       <c r="A29" s="6"/>
       <c r="C29" s="8">
         <v>28</v>
@@ -2901,17 +2215,13 @@
       <c r="K29" s="10"/>
       <c r="L29" s="10"/>
       <c r="M29" s="10"/>
-      <c r="N29" s="9">
-        <v>1</v>
-      </c>
+      <c r="N29" s="9"/>
       <c r="O29" s="10"/>
       <c r="P29" s="13"/>
       <c r="Q29" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R29" s="16">
-        <v>0</v>
-      </c>
+      <c r="R29" s="16"/>
       <c r="S29" s="17"/>
       <c r="T29" s="17"/>
       <c r="U29" s="13"/>
@@ -2931,7 +2241,7 @@
       <c r="AI29" s="19"/>
       <c r="AJ29" s="19"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1" spans="1:36">
+    <row r="30" spans="1:36" ht="15.75" customHeight="1">
       <c r="A30" s="6"/>
       <c r="C30" s="8">
         <v>29</v>
@@ -2950,17 +2260,13 @@
       <c r="K30" s="10"/>
       <c r="L30" s="10"/>
       <c r="M30" s="10"/>
-      <c r="N30" s="9">
-        <v>1</v>
-      </c>
+      <c r="N30" s="9"/>
       <c r="O30" s="10"/>
       <c r="P30" s="13"/>
       <c r="Q30" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R30" s="16">
-        <v>0</v>
-      </c>
+      <c r="R30" s="16"/>
       <c r="S30" s="17"/>
       <c r="T30" s="17"/>
       <c r="U30" s="13"/>
@@ -2980,7 +2286,7 @@
       <c r="AI30" s="19"/>
       <c r="AJ30" s="19"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1" spans="1:36">
+    <row r="31" spans="1:36" ht="15.75" customHeight="1">
       <c r="A31" s="6"/>
       <c r="C31" s="8">
         <v>30</v>
@@ -2999,17 +2305,13 @@
       <c r="K31" s="10"/>
       <c r="L31" s="10"/>
       <c r="M31" s="10"/>
-      <c r="N31" s="9">
-        <v>1</v>
-      </c>
+      <c r="N31" s="9"/>
       <c r="O31" s="10"/>
       <c r="P31" s="13"/>
       <c r="Q31" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R31" s="16">
-        <v>0</v>
-      </c>
+      <c r="R31" s="16"/>
       <c r="S31" s="17"/>
       <c r="T31" s="17"/>
       <c r="U31" s="13"/>
@@ -3029,7 +2331,7 @@
       <c r="AI31" s="19"/>
       <c r="AJ31" s="19"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1" spans="1:36">
+    <row r="32" spans="1:36" ht="15.75" customHeight="1">
       <c r="A32" s="6"/>
       <c r="C32" s="8">
         <v>31</v>
@@ -3048,17 +2350,13 @@
       <c r="K32" s="10"/>
       <c r="L32" s="10"/>
       <c r="M32" s="10"/>
-      <c r="N32" s="9">
-        <v>1</v>
-      </c>
+      <c r="N32" s="9"/>
       <c r="O32" s="10"/>
       <c r="P32" s="13"/>
       <c r="Q32" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R32" s="16">
-        <v>0</v>
-      </c>
+      <c r="R32" s="16"/>
       <c r="S32" s="17"/>
       <c r="T32" s="17"/>
       <c r="U32" s="13"/>
@@ -3078,7 +2376,7 @@
       <c r="AI32" s="19"/>
       <c r="AJ32" s="19"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1" spans="1:36">
+    <row r="33" spans="1:36" ht="15.75" customHeight="1">
       <c r="A33" s="6"/>
       <c r="C33" s="8">
         <v>32</v>
@@ -3097,17 +2395,13 @@
       <c r="K33" s="10"/>
       <c r="L33" s="10"/>
       <c r="M33" s="10"/>
-      <c r="N33" s="9">
-        <v>1</v>
-      </c>
+      <c r="N33" s="9"/>
       <c r="O33" s="10"/>
       <c r="P33" s="13"/>
       <c r="Q33" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R33" s="16">
-        <v>0</v>
-      </c>
+      <c r="R33" s="16"/>
       <c r="S33" s="17"/>
       <c r="T33" s="17"/>
       <c r="U33" s="13"/>
@@ -3127,7 +2421,7 @@
       <c r="AI33" s="19"/>
       <c r="AJ33" s="19"/>
     </row>
-    <row r="34" ht="15.75" customHeight="1" spans="1:36">
+    <row r="34" spans="1:36" ht="15.75" customHeight="1">
       <c r="A34" s="6"/>
       <c r="C34" s="8">
         <v>33</v>
@@ -3146,17 +2440,13 @@
       <c r="K34" s="10"/>
       <c r="L34" s="10"/>
       <c r="M34" s="10"/>
-      <c r="N34" s="9">
-        <v>1</v>
-      </c>
+      <c r="N34" s="9"/>
       <c r="O34" s="10"/>
       <c r="P34" s="13"/>
       <c r="Q34" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R34" s="16">
-        <v>0</v>
-      </c>
+      <c r="R34" s="16"/>
       <c r="S34" s="17"/>
       <c r="T34" s="17"/>
       <c r="U34" s="13"/>
@@ -3176,7 +2466,7 @@
       <c r="AI34" s="19"/>
       <c r="AJ34" s="19"/>
     </row>
-    <row r="35" ht="15.75" customHeight="1" spans="1:36">
+    <row r="35" spans="1:36" ht="15.75" customHeight="1">
       <c r="A35" s="6"/>
       <c r="C35" s="8">
         <v>34</v>
@@ -3195,17 +2485,13 @@
       <c r="K35" s="10"/>
       <c r="L35" s="10"/>
       <c r="M35" s="10"/>
-      <c r="N35" s="9">
-        <v>1</v>
-      </c>
+      <c r="N35" s="9"/>
       <c r="O35" s="10"/>
       <c r="P35" s="13"/>
       <c r="Q35" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R35" s="16">
-        <v>0</v>
-      </c>
+      <c r="R35" s="16"/>
       <c r="S35" s="17"/>
       <c r="T35" s="17"/>
       <c r="U35" s="13"/>
@@ -3225,7 +2511,7 @@
       <c r="AI35" s="19"/>
       <c r="AJ35" s="19"/>
     </row>
-    <row r="36" ht="15.75" customHeight="1" spans="1:36">
+    <row r="36" spans="1:36" ht="15.75" customHeight="1">
       <c r="A36" s="6"/>
       <c r="C36" s="8">
         <v>35</v>
@@ -3244,17 +2530,13 @@
       <c r="K36" s="10"/>
       <c r="L36" s="10"/>
       <c r="M36" s="10"/>
-      <c r="N36" s="9">
-        <v>1</v>
-      </c>
+      <c r="N36" s="9"/>
       <c r="O36" s="10"/>
       <c r="P36" s="13"/>
       <c r="Q36" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R36" s="16">
-        <v>0</v>
-      </c>
+      <c r="R36" s="16"/>
       <c r="S36" s="17"/>
       <c r="T36" s="17"/>
       <c r="U36" s="13"/>
@@ -3274,7 +2556,7 @@
       <c r="AI36" s="19"/>
       <c r="AJ36" s="19"/>
     </row>
-    <row r="37" ht="15.75" customHeight="1" spans="1:36">
+    <row r="37" spans="1:36" ht="15.75" customHeight="1">
       <c r="A37" s="6"/>
       <c r="C37" s="8">
         <v>36</v>
@@ -3293,17 +2575,13 @@
       <c r="K37" s="10"/>
       <c r="L37" s="10"/>
       <c r="M37" s="10"/>
-      <c r="N37" s="9">
-        <v>1</v>
-      </c>
+      <c r="N37" s="9"/>
       <c r="O37" s="10"/>
       <c r="P37" s="13"/>
       <c r="Q37" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R37" s="16">
-        <v>0</v>
-      </c>
+      <c r="R37" s="16"/>
       <c r="S37" s="17"/>
       <c r="T37" s="17"/>
       <c r="U37" s="13"/>
@@ -3323,7 +2601,7 @@
       <c r="AI37" s="19"/>
       <c r="AJ37" s="19"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1" spans="1:36">
+    <row r="38" spans="1:36" ht="15.75" customHeight="1">
       <c r="A38" s="6"/>
       <c r="C38" s="8">
         <v>37</v>
@@ -3342,17 +2620,13 @@
       <c r="K38" s="10"/>
       <c r="L38" s="10"/>
       <c r="M38" s="10"/>
-      <c r="N38" s="9">
-        <v>1</v>
-      </c>
+      <c r="N38" s="9"/>
       <c r="O38" s="10"/>
       <c r="P38" s="13"/>
       <c r="Q38" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R38" s="16">
-        <v>0</v>
-      </c>
+      <c r="R38" s="16"/>
       <c r="S38" s="17"/>
       <c r="T38" s="17"/>
       <c r="U38" s="13"/>
@@ -3372,7 +2646,7 @@
       <c r="AI38" s="19"/>
       <c r="AJ38" s="19"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1" spans="1:36">
+    <row r="39" spans="1:36" ht="15.75" customHeight="1">
       <c r="A39" s="6"/>
       <c r="C39" s="8">
         <v>38</v>
@@ -3391,17 +2665,13 @@
       <c r="K39" s="10"/>
       <c r="L39" s="10"/>
       <c r="M39" s="10"/>
-      <c r="N39" s="9">
-        <v>1</v>
-      </c>
+      <c r="N39" s="9"/>
       <c r="O39" s="10"/>
       <c r="P39" s="13"/>
       <c r="Q39" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R39" s="16">
-        <v>0</v>
-      </c>
+      <c r="R39" s="16"/>
       <c r="S39" s="17"/>
       <c r="T39" s="17"/>
       <c r="U39" s="13"/>
@@ -3421,7 +2691,7 @@
       <c r="AI39" s="19"/>
       <c r="AJ39" s="19"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1" spans="1:36">
+    <row r="40" spans="1:36" ht="15.75" customHeight="1">
       <c r="A40" s="6"/>
       <c r="C40" s="8">
         <v>39</v>
@@ -3440,17 +2710,13 @@
       <c r="K40" s="10"/>
       <c r="L40" s="10"/>
       <c r="M40" s="10"/>
-      <c r="N40" s="9">
-        <v>1</v>
-      </c>
+      <c r="N40" s="9"/>
       <c r="O40" s="10"/>
       <c r="P40" s="13"/>
       <c r="Q40" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R40" s="16">
-        <v>0</v>
-      </c>
+      <c r="R40" s="16"/>
       <c r="S40" s="17"/>
       <c r="T40" s="17"/>
       <c r="U40" s="13"/>
@@ -3470,7 +2736,7 @@
       <c r="AI40" s="19"/>
       <c r="AJ40" s="19"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1" spans="1:36">
+    <row r="41" spans="1:36" ht="15.75" customHeight="1">
       <c r="A41" s="6"/>
       <c r="C41" s="8">
         <v>40</v>
@@ -3489,17 +2755,13 @@
       <c r="K41" s="10"/>
       <c r="L41" s="10"/>
       <c r="M41" s="10"/>
-      <c r="N41" s="9">
-        <v>1</v>
-      </c>
+      <c r="N41" s="9"/>
       <c r="O41" s="10"/>
       <c r="P41" s="13"/>
       <c r="Q41" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R41" s="16">
-        <v>0</v>
-      </c>
+      <c r="R41" s="16"/>
       <c r="S41" s="17"/>
       <c r="T41" s="17"/>
       <c r="U41" s="13"/>
@@ -3519,7 +2781,7 @@
       <c r="AI41" s="19"/>
       <c r="AJ41" s="19"/>
     </row>
-    <row r="42" ht="15.75" customHeight="1" spans="1:36">
+    <row r="42" spans="1:36" ht="15.75" customHeight="1">
       <c r="A42" s="6"/>
       <c r="C42" s="8">
         <v>41</v>
@@ -3538,17 +2800,13 @@
       <c r="K42" s="10"/>
       <c r="L42" s="10"/>
       <c r="M42" s="10"/>
-      <c r="N42" s="9">
-        <v>1</v>
-      </c>
+      <c r="N42" s="9"/>
       <c r="O42" s="10"/>
       <c r="P42" s="13"/>
       <c r="Q42" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R42" s="16">
-        <v>0</v>
-      </c>
+      <c r="R42" s="16"/>
       <c r="S42" s="17"/>
       <c r="T42" s="17"/>
       <c r="U42" s="13"/>
@@ -3568,7 +2826,7 @@
       <c r="AI42" s="19"/>
       <c r="AJ42" s="19"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1" spans="1:36">
+    <row r="43" spans="1:36" ht="15.75" customHeight="1">
       <c r="A43" s="6"/>
       <c r="C43" s="8">
         <v>42</v>
@@ -3587,17 +2845,13 @@
       <c r="K43" s="10"/>
       <c r="L43" s="10"/>
       <c r="M43" s="10"/>
-      <c r="N43" s="9">
-        <v>1</v>
-      </c>
+      <c r="N43" s="9"/>
       <c r="O43" s="10"/>
       <c r="P43" s="13"/>
       <c r="Q43" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R43" s="16">
-        <v>0</v>
-      </c>
+      <c r="R43" s="16"/>
       <c r="S43" s="17"/>
       <c r="T43" s="17"/>
       <c r="U43" s="13"/>
@@ -3617,7 +2871,7 @@
       <c r="AI43" s="19"/>
       <c r="AJ43" s="19"/>
     </row>
-    <row r="44" ht="15.75" customHeight="1" spans="1:36">
+    <row r="44" spans="1:36" ht="15.75" customHeight="1">
       <c r="A44" s="6"/>
       <c r="C44" s="8">
         <v>43</v>
@@ -3636,17 +2890,13 @@
       <c r="K44" s="10"/>
       <c r="L44" s="10"/>
       <c r="M44" s="10"/>
-      <c r="N44" s="9">
-        <v>1</v>
-      </c>
+      <c r="N44" s="9"/>
       <c r="O44" s="10"/>
       <c r="P44" s="13"/>
       <c r="Q44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R44" s="16">
-        <v>0</v>
-      </c>
+      <c r="R44" s="16"/>
       <c r="S44" s="17"/>
       <c r="T44" s="17"/>
       <c r="U44" s="13"/>
@@ -3666,7 +2916,7 @@
       <c r="AI44" s="19"/>
       <c r="AJ44" s="19"/>
     </row>
-    <row r="45" ht="15.75" customHeight="1" spans="1:36">
+    <row r="45" spans="1:36" ht="15.75" customHeight="1">
       <c r="A45" s="6"/>
       <c r="C45" s="8">
         <v>44</v>
@@ -3685,17 +2935,13 @@
       <c r="K45" s="10"/>
       <c r="L45" s="10"/>
       <c r="M45" s="10"/>
-      <c r="N45" s="9">
-        <v>1</v>
-      </c>
+      <c r="N45" s="9"/>
       <c r="O45" s="10"/>
       <c r="P45" s="13"/>
       <c r="Q45" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R45" s="16">
-        <v>0</v>
-      </c>
+      <c r="R45" s="16"/>
       <c r="S45" s="17"/>
       <c r="T45" s="17"/>
       <c r="U45" s="13"/>
@@ -3715,7 +2961,7 @@
       <c r="AI45" s="19"/>
       <c r="AJ45" s="19"/>
     </row>
-    <row r="46" ht="15.75" customHeight="1" spans="1:36">
+    <row r="46" spans="1:36" ht="15.75" customHeight="1">
       <c r="A46" s="6"/>
       <c r="C46" s="8">
         <v>45</v>
@@ -3734,17 +2980,13 @@
       <c r="K46" s="10"/>
       <c r="L46" s="10"/>
       <c r="M46" s="10"/>
-      <c r="N46" s="9">
-        <v>1</v>
-      </c>
+      <c r="N46" s="9"/>
       <c r="O46" s="10"/>
       <c r="P46" s="13"/>
       <c r="Q46" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R46" s="16">
-        <v>0</v>
-      </c>
+      <c r="R46" s="16"/>
       <c r="S46" s="17"/>
       <c r="T46" s="17"/>
       <c r="U46" s="13"/>
@@ -3764,7 +3006,7 @@
       <c r="AI46" s="19"/>
       <c r="AJ46" s="19"/>
     </row>
-    <row r="47" ht="15.75" customHeight="1" spans="1:36">
+    <row r="47" spans="1:36" ht="15.75" customHeight="1">
       <c r="A47" s="6"/>
       <c r="C47" s="8">
         <v>46</v>
@@ -3783,17 +3025,13 @@
       <c r="K47" s="10"/>
       <c r="L47" s="10"/>
       <c r="M47" s="10"/>
-      <c r="N47" s="9">
-        <v>1</v>
-      </c>
+      <c r="N47" s="9"/>
       <c r="O47" s="10"/>
       <c r="P47" s="13"/>
       <c r="Q47" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R47" s="16">
-        <v>0</v>
-      </c>
+      <c r="R47" s="16"/>
       <c r="S47" s="17"/>
       <c r="T47" s="17"/>
       <c r="U47" s="13"/>
@@ -3813,7 +3051,7 @@
       <c r="AI47" s="19"/>
       <c r="AJ47" s="19"/>
     </row>
-    <row r="48" ht="15.75" customHeight="1" spans="1:36">
+    <row r="48" spans="1:36" ht="15.75" customHeight="1">
       <c r="A48" s="6"/>
       <c r="C48" s="8">
         <v>47</v>
@@ -3832,17 +3070,13 @@
       <c r="K48" s="10"/>
       <c r="L48" s="10"/>
       <c r="M48" s="10"/>
-      <c r="N48" s="9">
-        <v>1</v>
-      </c>
+      <c r="N48" s="9"/>
       <c r="O48" s="10"/>
       <c r="P48" s="13"/>
       <c r="Q48" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R48" s="16">
-        <v>0</v>
-      </c>
+      <c r="R48" s="16"/>
       <c r="S48" s="17"/>
       <c r="T48" s="17"/>
       <c r="U48" s="13"/>
@@ -3862,7 +3096,7 @@
       <c r="AI48" s="19"/>
       <c r="AJ48" s="19"/>
     </row>
-    <row r="49" ht="15.75" customHeight="1" spans="1:36">
+    <row r="49" spans="1:41" ht="15.75" customHeight="1">
       <c r="A49" s="6"/>
       <c r="C49" s="8">
         <v>48</v>
@@ -3881,17 +3115,13 @@
       <c r="K49" s="10"/>
       <c r="L49" s="10"/>
       <c r="M49" s="10"/>
-      <c r="N49" s="9">
-        <v>1</v>
-      </c>
+      <c r="N49" s="9"/>
       <c r="O49" s="10"/>
       <c r="P49" s="13"/>
       <c r="Q49" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R49" s="16">
-        <v>0</v>
-      </c>
+      <c r="R49" s="16"/>
       <c r="S49" s="17"/>
       <c r="T49" s="17"/>
       <c r="U49" s="13"/>
@@ -3911,7 +3141,7 @@
       <c r="AI49" s="19"/>
       <c r="AJ49" s="19"/>
     </row>
-    <row r="50" ht="15.75" customHeight="1" spans="1:36">
+    <row r="50" spans="1:41" ht="15.75" customHeight="1">
       <c r="A50" s="6"/>
       <c r="C50" s="8">
         <v>49</v>
@@ -3930,17 +3160,13 @@
       <c r="K50" s="10"/>
       <c r="L50" s="10"/>
       <c r="M50" s="10"/>
-      <c r="N50" s="9">
-        <v>1</v>
-      </c>
+      <c r="N50" s="9"/>
       <c r="O50" s="10"/>
       <c r="P50" s="13"/>
       <c r="Q50" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R50" s="16">
-        <v>0</v>
-      </c>
+      <c r="R50" s="16"/>
       <c r="S50" s="17"/>
       <c r="T50" s="17"/>
       <c r="U50" s="13"/>
@@ -3960,7 +3186,7 @@
       <c r="AI50" s="19"/>
       <c r="AJ50" s="19"/>
     </row>
-    <row r="51" ht="15.75" customHeight="1" spans="1:36">
+    <row r="51" spans="1:41" ht="15.75" customHeight="1">
       <c r="A51" s="6"/>
       <c r="C51" s="8">
         <v>50</v>
@@ -3979,17 +3205,13 @@
       <c r="K51" s="10"/>
       <c r="L51" s="10"/>
       <c r="M51" s="10"/>
-      <c r="N51" s="9">
-        <v>1</v>
-      </c>
+      <c r="N51" s="9"/>
       <c r="O51" s="10"/>
       <c r="P51" s="13"/>
       <c r="Q51" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R51" s="16">
-        <v>0</v>
-      </c>
+      <c r="R51" s="16"/>
       <c r="S51" s="17"/>
       <c r="T51" s="17"/>
       <c r="U51" s="13"/>
@@ -4009,7 +3231,7 @@
       <c r="AI51" s="19"/>
       <c r="AJ51" s="19"/>
     </row>
-    <row r="52" ht="15.75" customHeight="1" spans="1:36">
+    <row r="52" spans="1:41" ht="15.75" customHeight="1">
       <c r="A52" s="6"/>
       <c r="C52" s="8">
         <v>51</v>
@@ -4028,17 +3250,13 @@
       <c r="K52" s="10"/>
       <c r="L52" s="10"/>
       <c r="M52" s="10"/>
-      <c r="N52" s="9">
-        <v>1</v>
-      </c>
+      <c r="N52" s="9"/>
       <c r="O52" s="10"/>
       <c r="P52" s="13"/>
       <c r="Q52" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="R52" s="16">
-        <v>0</v>
-      </c>
+      <c r="R52" s="16"/>
       <c r="S52" s="17"/>
       <c r="T52" s="17"/>
       <c r="U52" s="13"/>
@@ -4058,9 +3276,9 @@
       <c r="AI52" s="19"/>
       <c r="AJ52" s="19"/>
     </row>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1" spans="38:41">
+    <row r="53" spans="1:41" ht="15.75" customHeight="1"/>
+    <row r="54" spans="1:41" ht="15.75" customHeight="1"/>
+    <row r="55" spans="1:41" ht="15.75" customHeight="1">
       <c r="AL55" s="20" t="s">
         <v>37</v>
       </c>
@@ -4074,7 +3292,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="56" ht="15.75" customHeight="1" spans="38:41">
+    <row r="56" spans="1:41" ht="15.75" customHeight="1">
       <c r="AL56" s="23">
         <v>1</v>
       </c>
@@ -4091,7 +3309,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="57" ht="15.75" customHeight="1" spans="38:41">
+    <row r="57" spans="1:41" ht="15.75" customHeight="1">
       <c r="AL57" s="23">
         <v>2</v>
       </c>
@@ -4108,7 +3326,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="58" ht="15.75" customHeight="1" spans="38:41">
+    <row r="58" spans="1:41" ht="15.75" customHeight="1">
       <c r="AL58" s="23">
         <v>3</v>
       </c>
@@ -4125,7 +3343,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="59" ht="15.75" customHeight="1" spans="38:41">
+    <row r="59" spans="1:41" ht="15.75" customHeight="1">
       <c r="AL59" s="23">
         <v>4</v>
       </c>
@@ -4142,7 +3360,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="60" ht="15.75" customHeight="1" spans="38:41">
+    <row r="60" spans="1:41" ht="15.75" customHeight="1">
       <c r="AL60" s="23">
         <v>5</v>
       </c>
@@ -4159,7 +3377,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="61" ht="15.75" customHeight="1" spans="38:41">
+    <row r="61" spans="1:41" ht="15.75" customHeight="1">
       <c r="AL61" s="23">
         <v>6</v>
       </c>
@@ -4176,7 +3394,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="62" ht="15.75" customHeight="1" spans="38:41">
+    <row r="62" spans="1:41" ht="15.75" customHeight="1">
       <c r="AL62" s="23">
         <v>7</v>
       </c>
@@ -4193,7 +3411,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="63" ht="15.75" customHeight="1" spans="38:41">
+    <row r="63" spans="1:41" ht="15.75" customHeight="1">
       <c r="AL63" s="23">
         <v>8</v>
       </c>
@@ -4210,7 +3428,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="64" ht="15.75" customHeight="1" spans="38:41">
+    <row r="64" spans="1:41" ht="15.75" customHeight="1">
       <c r="AL64" s="23">
         <v>9</v>
       </c>
@@ -4227,7 +3445,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="65" ht="15.75" customHeight="1" spans="38:41">
+    <row r="65" spans="38:41" ht="15.75" customHeight="1">
       <c r="AL65" s="27">
         <v>10</v>
       </c>
@@ -4239,15 +3457,15 @@
         <f>LARGE(#REF!,10)</f>
         <v>#REF!</v>
       </c>
-      <c r="AO65" s="34" t="e">
+      <c r="AO65" s="32" t="e">
         <f>AN65/#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="66" ht="3.75" customHeight="1" spans="41:41">
-      <c r="AO66" s="35"/>
-    </row>
-    <row r="67" ht="15.75" customHeight="1" spans="38:41">
+    <row r="66" spans="38:41" ht="3.75" customHeight="1">
+      <c r="AO66" s="33"/>
+    </row>
+    <row r="67" spans="38:41" ht="15.75" customHeight="1">
       <c r="AL67" s="8">
         <v>11</v>
       </c>
@@ -4258,37 +3476,37 @@
         <f>AN68-SUM(AN56:AN65)</f>
         <v>#REF!</v>
       </c>
-      <c r="AO67" s="36" t="e">
+      <c r="AO67" s="34" t="e">
         <f>AN67/#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="68" ht="15.75" customHeight="1" spans="38:41">
-      <c r="AL68" s="31" t="s">
+    <row r="68" spans="38:41" ht="15.75" customHeight="1">
+      <c r="AL68" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="AM68" s="32"/>
-      <c r="AN68" s="33" t="e">
+      <c r="AM68" s="37"/>
+      <c r="AN68" s="31" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="AO68" s="37" t="e">
+      <c r="AO68" s="35" t="e">
         <f>AN68/#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
+    <row r="69" spans="38:41" ht="15.75" customHeight="1"/>
+    <row r="70" spans="38:41" ht="15.75" customHeight="1"/>
+    <row r="71" spans="38:41" ht="15.75" customHeight="1"/>
+    <row r="72" spans="38:41" ht="15.75" customHeight="1"/>
+    <row r="73" spans="38:41" ht="15.75" customHeight="1"/>
+    <row r="74" spans="38:41" ht="15.75" customHeight="1"/>
+    <row r="75" spans="38:41" ht="15.75" customHeight="1"/>
+    <row r="76" spans="38:41" ht="15.75" customHeight="1"/>
+    <row r="77" spans="38:41" ht="15.75" customHeight="1"/>
+    <row r="78" spans="38:41" ht="15.75" customHeight="1"/>
+    <row r="79" spans="38:41" ht="15.75" customHeight="1"/>
+    <row r="80" spans="38:41" ht="15.75" customHeight="1"/>
     <row r="81" ht="15.75" customHeight="1"/>
     <row r="82" ht="15.75" customHeight="1"/>
     <row r="83" ht="15.75" customHeight="1"/>
@@ -5214,21 +4432,21 @@
     <mergeCell ref="AL68:AM68"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:B2">
-    <cfRule type="containsText" dxfId="0" priority="3" operator="between" text="not ">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="not ">
       <formula>NOT(ISERROR(SEARCH("not ",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52:B52">
-    <cfRule type="containsText" dxfId="0" priority="2" operator="between" text="not ">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="not ">
       <formula>NOT(ISERROR(SEARCH("not ",A52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:B51">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="between" text="not ">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="not ">
       <formula>NOT(ISERROR(SEARCH("not ",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="9">
+  <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2">
       <formula1>tabel_dept</formula1>
     </dataValidation>
@@ -5241,24 +4459,41 @@
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F52 H2:H52 O2:O52">
       <formula1>INDIRECT(#REF!)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:I52">
-      <formula1>'[1]#REF'!$W$26:$W$32</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K2:K52">
       <formula1>T_impdom</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="T2:T52 V2:V52">
-      <formula1>'[1]#REF'!$Y$51:$Y$70</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="S2:S52">
-      <formula1>'[1]#REF'!$Y$17:$Y$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="X2:X52">
-      <formula1>'[1]#REF'!$X$73:$X$75</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'[1]#REF'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2:I52</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'[1]#REF'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>T2:T52 V2:V52</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'[1]#REF'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>S2:S52</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'[1]#REF'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>X2:X52</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>